<commit_message>
Commit to create table for developing export code and prints of login an sign-up funcionalities.
</commit_message>
<xml_diff>
--- a/documents/prototypes/export_codes_prototype.xlsx
+++ b/documents/prototypes/export_codes_prototype.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2c3ffd89d078c25/homogenise/documents/prototype/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2c3ffd89d078c25/homogenise/documents/prototypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="92" documentId="8_{849BD15B-8617-42BB-B1E1-E50B9B0B7BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ECF9E2F-2ECB-4C37-8BBE-534024A37F65}"/>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +157,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -299,7 +305,7 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,13 +321,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +510,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C57C855-AEE9-91F8-A69C-952419576343}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -612,13 +618,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>19049</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>9524</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
@@ -688,7 +694,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30233808-69FA-A27F-E8FE-98CD9A3EE8D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -724,6 +730,10 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1264,10 +1274,10 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="12"/>
+      <c r="H18" s="13"/>
       <c r="I18" s="1"/>
       <c r="J18" s="6"/>
       <c r="L18" s="10" t="s">
@@ -1371,8 +1381,8 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="6"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" s="5"/>
@@ -1383,7 +1393,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="6"/>
-      <c r="L26" s="13"/>
+      <c r="L26" s="11"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="5"/>

</xml_diff>